<commit_message>
update some perl result.
</commit_message>
<xml_diff>
--- a/test/perl_output/array_formula.xlsx
+++ b/test/perl_output/array_formula.xlsx
@@ -383,6 +383,9 @@
       </c>
     </row>
     <row r="6" spans="1:3">
+      <c r="A6">
+        <v>0</v>
+      </c>
       <c r="B6">
         <v>2</v>
       </c>
@@ -391,6 +394,9 @@
       </c>
     </row>
     <row r="7" spans="1:3">
+      <c r="A7">
+        <v>0</v>
+      </c>
       <c r="B7">
         <v>3</v>
       </c>

</xml_diff>